<commit_message>
Edit UI, Don't decrypt packet with CODE value 400, shorten syntax in Global.cs, minor edition at login and register forms
</commit_message>
<xml_diff>
--- a/ClientDictApp/records/records.xlsx
+++ b/ClientDictApp/records/records.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\OneDrive\Máy tính\Assignments\Network Programming\nwfinal\DictApp\ClientDictApp\records\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66FD1FC9-3BC6-4B57-A0A2-A6C9AE90D9B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6079A8A-2BEE-4F40-B84B-D4810B6C024D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-100" yWindow="-100" windowWidth="21467" windowHeight="12163" xr2:uid="{73BC7031-A1D3-46B7-8448-72885C71CADC}"/>
+    <workbookView xWindow="5317" yWindow="3733" windowWidth="15951" windowHeight="8230" xr2:uid="{73BC7031-A1D3-46B7-8448-72885C71CADC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="36">
   <si>
     <t>Note</t>
   </si>
@@ -45,6 +45,594 @@
   </si>
   <si>
     <t>User</t>
+  </si>
+  <si>
+    <t>cat</t>
+  </si>
+  <si>
+    <t>�ng tục) người kỳ quặc; thằng cha, gã_x000D_
+=a knowing card+ một thằng cha láu_x000D_
+=a queer card+ một thằng cha kỳ quặc_x000D_
+!to have a card up one's sleeve_x000D_
+- còn nắm bài chủ trong tay; có kế dự phòng_x000D_
+!to have (hold) the cards in one's hands_x000D_
+- có tất cả bài chủ trong tay; (nghĩa bóng) có tất cả yếu tố thắng lợi trong tay_x000D_
+!house of cards_x000D_
+- (xem) house_x000D_
+!on (in) the cards_x000D_
+- có thể, có lẽ_x000D_
+!one's best (trump) cards_x000D_
+- lý lẽ vững nhất; lá bài chủ (nghĩa bóng)_x000D_
+!to play one's card well_x000D_
+- chơi nước bài hay ((nghĩa đen) &amp; (nghĩa bóng))_x000D_
+!to play a sure card_x000D_
+- chơi nước chắc ((nghĩa đen) &amp; (nghĩa bóng))_x000D_
+!to play a wrong card_x000D_
+- chơi nước bài bớ, chơi nước bài sai lầm ((nghĩa đen) &amp; (nghĩa bóng))_x000D_
+!to play (lay, place) one's card on the table_x000D_
+- nói rõ hết ý định, nói rõ hết kế hoạch không cần úp mở giấu giếm_x000D_
+!to show one's card_x000D_
+- để lộ kế hoạch_x000D_
+!to speak by the card_x000D_
+- nói rành rọt, nói chính xác_x000D_
+!that's the card_x000D_
+- (thông tục) đúng thế, thế là đúng, thế là phải_x000D_
+!to throw (fling) up one's card_x000D_
+- bỏ cuộc, chịu thua</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>�n phòng đông nghịt khán giả_x000D_
+_x000D_
+@chocolate /'tʃɔkəlit/_x000D_
+*  danh từ_x000D_
+- sôcôla_x000D_
+- kẹo sôcôla_x000D_
+- nước sôcôla_x000D_
+- màu sôcôla_x000D_
+*  tính từ_x000D_
+- có màu sôcôla_x000D_
+_x000D_
+@chocolate soldier /'tʃɔkəlit'souldʤə/_x000D_
+*  danh từ_x000D_
+- lính cậu, lính không làm nhiệm vụ chiến đấu_x000D_
+_x000D_
+@choice /tʃɔis/_x000D_
+*  danh từ_x000D_
+- sự lựa, sự chọn, sự lựa chọn_x000D_
+=choice of words+ sự chọn từ_x000D_
+=to make one's choice of+ chọn, lựa chọn_x000D_
+=to take one's choice+ quyết định chọn một trong nhiều khả năng_x000D_
+=at choice+ tuỳ thích_x000D_
+=by (for</t>
+  </si>
+  <si>
+    <t>rock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+- lấy lại, thu đi, gỡ lại, chiếm lại, chuộc lại_x000D_
+=to regain consciousness+ tỉnh lại_x000D_
+- trở lại (nơi nào)_x000D_
+=to regain one's home+ trở lại gia đình_x000D_
+_x000D_
+@regal /'ri:gəl/_x000D_
+*  tính từ_x000D_
+- (thuộc) vua chúa; xứng với vua chúa; như vua chúa_x000D_
+=regal power+ vương quyền_x000D_
+=to live in regal splendour+ sống huy hoàng như một ông vua, sống đế vương_x000D_
+_x000D_
+@regale /ri'geil/_x000D_
+*  danh từ_x000D_
+- bữa tiệc, bữa ăn có món ăn quý_x000D_
+- (từ hiếm,nghĩa hiếm) món ăn ngon_x000D_
+*  ngoại động từ_x000D_
+- ((thường)(mỉa mai)) đâi tiệc, thết đâi, đãi rất hậu_x000D_
+=to regale someone with a good meal+ thết ai một bữa ăn ngon_x000D_
+- làm thích thú, làm khoái trá (vẻ đẹp, nhạc...)_x000D_
+- chè chén thoả thích, hưởng cho kỳ thoả, thưởng thức một cách khoái trá_x000D_
+=to regale oneself with beer+ uống bia thoả thích_x000D_
+*  nội động từ_x000D_
+- chè chén thoả thích_x000D_
+- lấy làm khoái trá (về cái gì...)_x000D_
+_x000D_
+@regalement /ri'geilmənt/_x000D_
+*  danh từ_x000D_
+- sự thết đâi, sự đãi hậu_x000D_
+- sự chè chén thoả thích_x000D_
+- sự thưởng thức khoái trá_x000D_
+_x000D_
+@regalia /ri'geiljə/_x000D_
+*  danh từ số nhiều_x000D_
+- những biểu chương của nhà vua_x000D_
+- những dấu hiệu tựng trưng của một </t>
+  </si>
+  <si>
+    <t>lan</t>
+  </si>
+  <si>
+    <t>this</t>
+  </si>
+  <si>
+    <t>�ng sách)_x000D_
+_x000D_
+@superable /'sju:pərəbl/_x000D_
+*  tính từ_x000D_
+- có thể vượt qua được, có thể khắc phục được_x000D_
+_x000D_
+@superabound /,sju:pərə'baund/_x000D_
+*  nội động từ_x000D_
+- thừa thãi quá, dư dật quá, dồi dào quá_x000D_
+_x000D_
+@superabundance /,sju:pərə'bʌndəns/_x000D_
+*  danh từ_x000D_
+- sự rất mực thừa thãi, sự rất mực dư thừa, sự rất mực dồi dào_x000D_
+_x000D_
+@superabundant /,sju:pərə'bʌndənt/_x000D_
+*  tính từ_x000D_
+- rất mực thừa thãi, rất mực dư dật, rất mực dồi dào_x000D_
+_x000D_
+@superadd /,sju:pər'æd/_x000D_
+*  ngoại động từ_x000D_
+- thêm vào nhiều quá_x000D_
+_x000D_
+@superaddition /,sju:pərə'diʃn/_x000D_
+*  danh từ_x000D_
+- sự thêm vào nhiều quá, sự gia tăng nhiều quá_x000D_
+_x000D_
+@superanal /,sju:pə'reinəl/_x000D_
+*  tính từ_x000D_
+- (giải phẫu) trên hậu môn_x000D_
+_x000D_
+@superangelic /,sju:pər�</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@cat /kæt/
+*  danh từ
+- con mèo
+- (động vật học) thú thuộc giống mèo (sư tử, hổ, báo...)
+- mụ đàn bà nanh ác; đứa bé hay cào cấu
+- (hàng hải) đòn kéo neo ((cũng) cat head)
+- roi chín dài (để tra tấn) ((cũng) cat o-nine-tails)
+- con khăng (để chơi đanh khăng)
+!all cats are grey in the dark (in the night)
+- (tục ngữ) tắt đèn nhà ngói cũng như nhà tranh
+!cat in the pan (cat-in-the-pan)
+- kẻ trở mặt, kẻ phản bội
+!the cat is out the bag
+- điều bí mật đã bị tiết lộ rồi
+!fat cat
+- (từ Mỹ,nghĩa Mỹ),  (từ lóng) tư bản kếch xù, tài phiệt
+!to fight like Kilkemy cats
+- giết hại lẫn nhau
+!to let the cat out of the bag
+- (xem) let
+!it rains cats and dogs
+- (xem) rain
+!to see which way the cat jumps; to wait for the cat to jump
+- đợi gió xoay chiều, đợi gió chiều nào thì theo chiều ấy
+!to room to swing a cat
+- (xem) room
+!to turn cat in the pan
+- trở mặt; thay đổi ý kiến (lúc lâm nguy); phản hồi
+*  ngoại động từ
+- (hàng hải) kéo (neo) lên đòn kéo neo
+- đánh bằng roi chín dài
+*  nội động từ
+- (thông tục) nôn mửa
+</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@country /'kʌntri/
+*  danh từ
+- nước, quốc gia
+- đất nước, tổ quốc, quê hương, xứ sở
+- nhân dân (một nước)
+- số ít vùng, xứ, miền; (nghĩa bóng) địa hạt, lĩnh vực
+=densely wooded country+ vùng cây cối rậm rạp
+=this is unknown country to me+ đó là một vùng mà tôi chưa đi qua; (nghĩa bóng) đó là một lĩnh vực xa lạ đối với tôi
+- số ít nông thôn, thôn dã
+=to live in the country+ sống ở nông thôn
+=the country life+ đời sống (cách sinh hoạt) ở nông thôn
+!to go (appeal) to the country
+- giải tán quốc hội và tổ chức bầu lại
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@this /ðis/
+*  tính từ chỉ định,  số nhiều these
+- này
+=this box+ cái hộp này
+=this way+ lối này
+=by this time+ bây giờ, hiện nay, lúc này
+=this he has been ill these two months+ anh ấy ốm hai tháng nay
+=this day last year+ ngày này năm ngoái
+*  đại từ chỉ định,  số nhiều these
+- cái này, điều này, việc này
+=I don't like this+ tôi không thích cái này
+=will you have this or that?+ anh muốn cái này hay cái kia?
+- thế này
+=to it like this+ hãy làm việc dó như thế này
+!by this
+- bây giờ, hiện nay, lúc này
+!with this; at this
+- như thế này, cơ sự đã thế này, vào lúc sự việc thế này
+*  phó từ
+- như thế này
+=this far+ xa thế này; tới đây, tới bây giờ
+=it was this big+ nó to như thế này
+</t>
+  </si>
+  <si>
+    <t>dog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@dog /dɔg/
+*  danh từ
+- chó
+- chó săn
+- chó đực; chó sói đực ((cũng) dog wolf); cáo đực ((cũng) dog fox)
+- kẻ đê tiện, kẻ đáng khinh, đồ chó má; kẻ cắn cẩu cục cằn
+- gã, thằng cha
+=a sly dog+ thằng cha vận đỏ
+=Greater Dog+ (thiên văn học) chòm sao Đại-thiên-lang
+=Lesser Dog+ chòm sao Tiểu-thiên-lang
+- (số nhiều) vỉ lò (ở lò sưởi) ((cũng) fire dogs)
+- (kỹ thuật) móng kìm, cặp, móc ngoạm, gàu ngoạm
+- mống bão, ráng bão (ở chân trời) ((cũng) sea dog)
+- (như) dogfish
+!to be a dog in the manger
+- như chó già giữ xương; ích kỷ, không muốn ai dùng đến cái gì mình không cần đến
+!to die a dog's death
+!to die like a dog
+- chết khổ, chết sở, chết nhục nhã, chết như một con chó
+!dog and war
+- những sự tàn phá giết chóc của chiến tranh
+!every dog has his day
+- ai rồi cũng có lúc gặp vận; ai khó ba đời
+!to give a dog an ill name and hang him
+- muốn giết chó thì bảo là chó dại; không ưa thì dưa có giòi
+!to go to the dogs
+- thất cơ lỡ vận, khánh kiệt, xuống dốc ((nghĩa bóng))
+- sa đoạ
+!to help a lame dog over stile
+- giúp đỡ ai trong lúc khó khăn
+!to leaf a dog's life
+- sống một cuộc đời khổ như chó
+!to lead someone a dog's life
+- bắt ai sống một cuộc đời khổ cực
+!let sleeping dogs lie
+- (tục ngữ) đừng khêu gợi lại những chuyện đã êm thấm; đừng bới cứt ra mà ngửi
+!love me love my dog
+- yêu tôi thì hãy yêu cả những người thân của tôi
+!not even a dog's chance
+- không có chút may mắn nào
+!not to have a word to throw at the dog
+- lầm lì không mở miệng nói nửa lời; kiêu kỳ không thèm mở miệng nói nửa lời
+!to put on dog
+- (thông tục) làm bộ làm tịch, làm ra vẻ ta đây, làm ra vẻ ta đây quan trọng
+!it rains cats and dogs
+- (xem) rain
+!to take a hair of the dog that big you
+- (xem) hair
+!to throw to the dogs
+- vứt bỏ đi, quẳng đi (cho chó)
+*  ngoại động từ
+- theo nhùng nhằng, theo sát gót, bám sát (ai)
+=to dog someone's footsteps+ bám sát ai
+- (kỹ thuật) kẹp bằng kìm, cặp bằng móc ngoạm
+</t>
+  </si>
+  <si>
+    <t>young</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@young /jʌɳ/
+*  tính từ
+- trẻ, trẻ tuổi, thiếu niên, thanh niên
+=a young man+ một thanh niên
+=young people+ thanh niên
+=his (her) young woman (man)+ người yêu của nó
+=a young family+ gia đình có nhiều con nhỏ
+=a young person+ người đàn bà lạ trẻ tuổi thuộc tầng lớp dưới (trong ngôn ngữ những người ở của các gia đình tư sản quý tộc Anh)
+=the young person+ những người còn non trẻ ngây thơ cần giữ gìn không cho nghe (đọc) những điều tục tĩu
+- non
+=young tree+ cây non
+- (nghĩa bóng) non trẻ, trẻ tuổi
+=a young republic+ nước cộng hoà trẻ tuổi
+=he is young for his age+ nó còn non so với tuổi, nó trẻ hơn tuổi
+- (nghĩa bóng) non nớt, mới mẻ, chưa có kinh nghiệm
+=young in mind+ trí óc còn non nớt
+=young in bussiness+ chưa có kinh nghiệm kinh doanh
+- (nghĩa bóng) còn sớm, còn ở lúc ban đầu, chưa muộn, chưa quá, chưa già
+=the night is young yet+ đêm chưa khuya
+=young moon+ trăng non
+=autumn is still young+ thu hãy còn đang ở lúc đầu mùa
+- của tuổi trẻ, của thời thanh niên, của thời niên thiếu, (thuộc) thế hệ trẻ
+=young hope+ hy vọng của tuổi trẻ
+=in one's young days+ trong thời kỳ thanh xuân, trong lúc tuổi còn trẻ
+- (thông tục) con, nhỏ
+=young Smith+ thằng Xmít con, cậu Xmít
+*  danh từ
+- thú con, chim con (mới đẻ)
+=with young+ có chửa (thú)
+</t>
+  </si>
+  <si>
+    <t>bird</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@bird /bə:d/
+*  danh từ
+- con chim
+- (thông tục) gã, thằng cha
+=a queer bird+ thằng cha kỳ dị
+- (từ lóng) cô gái
+!a bird in the bush
+- điều mình không biết; điều không chắc chắn có
+!birds of a feather
+- những người giống tính nết nhau, những người cùng một giuộc
+!birds of a feather flock together
+- (tục ngữ) ngưu tầm ngưu, mã tầm mã
+!a bird in the hand
+- vật mình có chắc trong tay; điều mình chắc chắn
+!a bird in the hand is worth two in the bush
+- (tục ngữ) không nên thả mồi bắt bóng
+!bird of ill omen
+- người mang tin xấu
+- người không may, người gặp vận rủi
+!bird of passage
+- chim di trú; (nghĩa bóng) người nay đây mai đó
+!bird of peace
+- chim hoà bình, bồ câu
+!to get the bird
+- bị huýt sáo, bị la ó
+- bị đuổi đi
+!to give someone the bird
+- huýt sáo ai, la ó ai
+- đuổi ai, tống cổ ai đi
+!to kill two birds with one stone
+- một công đôi việc
+!little bird
+- người báo tin vô danh
+!old bird
+- (xem) old
+</t>
+  </si>
+  <si>
+    <t>fish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@fish /fiʃ/
+*  danh từ
+- cá
+=freshwater fish+ cá nước ngọt
+=salt-water fish+ cá nước mặn
+- cá, món cá
+- (thiên văn học) chòm sao Cá
+- người cắn câu, người bị mồi chài
+- con người gã (có cá tính đặc biệt)
+=a queer fish+ một con người (gã) kỳ quặc
+!all's fish that comes to his net
+- lớn bé, to nhỏ hắn quơ tất
+!to be as drunk as a fish
+- say bí tỉ
+!to be as mute as a fish
+- câm như hến
+!to drink like a fish
+- (xem) drink
+!to feed the fishes
+- chết đuối
+- bị say sóng
+!like a fish out of water
+- (xem) water
+!to have other fish to fly
+- có công việc khác quan trọng hơn
+!he who would catch fish must not mind getting wet
+- muốn ăn cá phải lội nước, muốn ăn hét phải đào giun
+!neither fish, fish, not good red herring
+- môn chẳng ra môn, khoai chẳng ra khoai
+!never fry a fish till it's caught
+- chưa làm vòng chớ vội mong ăn thịt
+!never offer to teach fish to swim
+- chớ nên múa rìu qua mắt thợ
+!a pretty kettle of fish
+- (xem) kettle
+!there's as good fish in the sea as ever came out of it
+- thừa mứa chứa chan, nhiều vô kể
+*  nội động từ
+- đánh cá, câu cá, bắt cá
+=to fish in the sea+ đánh cá ở biển
+- (+ for) tìm, mò (cái gì ở dưới nước)
+- (+ for) câu, moi những điều bí mật
+*  ngoại động từ
+- câu cá ở, đánh cá ở, bắt cá ở
+=to fish a river+ đánh cá ở sông
+- (hàng hải)
+=to fish the anchor+ nhổ neo
+- rút, lấy, kéo, moi
+=to fish something out of water+ kéo cái gì từ dưới nước lên
+- (từ hiếm,nghĩa hiếm) câu (cá), đánh (cá), bắt (cá), tìm (san hô...)
+=to fish a troud+ câu một con cá hồi
+!to fish out
+- đánh hết cá (ở ao...)
+- moi (ý kiến, bí mật)
+!to fish in troubled waters
+- lợi dụng đục nước béo cò
+*  danh từ
+- (hàng hải) miếng gỗ nẹp, miếng sắt nẹp (ở cột buồm, ở chỗ nối)
+- (ngành đường sắt) thanh nối ray ((cũng) fish plate)
+*  ngoại động từ
+- (hàng hải) nẹp (bằng gỗ hay sắt)
+- nối (đường ray) bằng thanh nối ray
+*  danh từ
+- (đánh bài) thẻ (bằng ngà... dùng thay tiền để đánh bài)
+</t>
+  </si>
+  <si>
+    <t>you</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@you /ju:/
+*  đại từ
+- anh, chị, ông, bà, ngài, ngươi, mày; các anh, các chị, các ông, các bà, các ngài, các người, chúng mày
+=you all know that...+ tất cả các anh đều biết rằng...
+=he spoke of you+ hắn ta nói về anh
+=if I were you+ nếu tôi là anh
+=you there what is your name?+ anh kia, tên anh là gì?
+- ai, người ta
+=you never can tell+ ai biết đâu được
+</t>
+  </si>
+  <si>
+    <t>super</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@super /'sju:pə/
+*  tính từ
+- (thông tục) thượng hảo hạng
+- vuông, (đo) diện tích (đơn vị đo) (không phải đo bề dài hay đo thể tích) ((cũng) superficial)
+- (từ lóng) cừ, chiến
+*  danh từ
+- (thông tục) kép phụ
+- người thừa, người không quan trọng
+- người giám thị, người quản lý
+- phim chính
+- hàng hoá thượng hảo hạng
+- vải lót hồ cứng (đóng sách)
+</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@high /hai/
+*  tính từ
+- cao
+=high mountain+ núi cao
+=high flight+ sự bay cao
+=high price+ giá cao
+=high speed+ tốc độ cao
+=high voice+ giọng cao
+=to have a high opinion of+ đánh giá cao
+- cao giá, đắt
+=corn is high+ lúa gạo đắt
+- lớn, trọng; tối cao, cao cấp; thượng, trên
+=high road+ đường cái
+=high crime+ trọng tội, tội lớn
+=High Court+ toà án tối cao
+=high antiquity+ thượng cổ
+=higher mathematics+ toán cao cấp
+=the higher classes+ tầng lớp thượng lưu, tầng lớp trên
+=the higher middle class+ tiểu tư sản lớp trên
+- cao quý, cao thượng, cao cả
+=high thoughts+ tư tưởng cao cả
+- mạnh, dữ dội, mãnh liệt, giận dữ
+=high wind+ gió mạnh
+=high fever+ sốt dữ dội, sốt cao
+=high words+ lời nói nặng
+- sang trọng, xa hoa
+=high living+ lối sống sang trọng xa hoa
+=high feeding+ sự ăn uống sang trọng
+- kiêu kỳ, kiêu căng, hách dịch
+=high look+ vẻ kiêu kỳ
+=high and mighty+ vô cùng kiêu ngạo
+- vui vẻ phấn khởi; hăng hái; dũng cảm
+=in high spirits+ vui vẻ phấn khới, phấn chấn
+=high spirit+ tinh thần dũng cảm
+- cực đoan
+=a high Tory+ đảng viên Bảo thủ cực đoan (ở Anh)
+- hơi có mùi (thối), hơi ôi
+=high game+ thịt thú săn để đã có hơi có mùi
+=high meat+ thịt hơi ôi
+- đúng giữa; đến lúc
+=high noon+ đúng giữa trưa
+=high summer+ đúng giữa mùa hạ
+=it's high time to go+ đã đến lúc phải đi, không thì muộn
+- (từ Mỹ,nghĩa Mỹ) (+ on) ngà ngà say
+!to mount (be on, get on, ride) the high horse
+- (xem) horse
+!high and dry
+- bị mắc cạn (tàu thuỷ)
+- (nghĩa bóng) xa rời thực tế, không biết gì đến việc xung quanh (người)
+!on the high ropes
+- (xem) rope
+!the Most High
+- Thượng đế
+!with a high hand
+- (xem) hand
+*  phó từ
+- cao, ở mức độ cao
+=to soar high in the sky+ bay vút lên cao trong bầu trời
+=to sing high+ hát cao giọng
+=prices run high+ giá cả lên cao
+- lớn
+=to plwy high+ (đánh bài) đánh lớn; đánh những quân bài cao
+- mạnh mẽ, dữ dội, mãnh liệt; giận dữ
+=the wind blows high+ gió thổi mạnh
+=words run high+ lời lẽ trở nên giận dữ
+- sang trọng, xa hoa
+=to live high+ sống sang trọng xa hoa
+*  danh từ
+- độ cao; điểm cao
+- quân bài cao nhất (đánh ra hay rút được)
+- nơi cao, trời cao
+=on high+ ở trên cao, ở trên trời
+</t>
+  </si>
+  <si>
+    <t>dream</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@dream /dri:m/
+*  danh từ
+- giấc mơ, giấc mộng
+=in a dream+ trong giấc mơ
+=to see a dream+ nằm mơ
+- sự mơ mộng, sự mơ màng, sự mộng tưởng
+=in a waking dream+ trong lúc mơ màng, trong lúc mơ mộng
+- điều mơ tưởng, điều mơ ước; điều kỳ ảo như trong giấc mơ
+=the dream of one's life+ điều mơ tưởng của đời mình
+*  động từ dreamt,  dreamed
+- mơ, nằm mơ thấy
+=he must have dreamt it+ hẳn là nó nằm mơ thấy điều đó
+- mơ màng, mơ mộng, vẩn vơ
+=to dream away one's time+ mơ mộng vẩn vơ hết thì giờ
+- (thường),  phủ định tưởng tượng, mơ tưởng; nghĩ rằng, tưởng rằng, có ý niệm rằng
+=I never dream of doing such a thing+ tôi không hề bao giờ nghĩ đến chuyện làm một điều như thế
+=to dream of something+ mơ tưởng tới cái gì
+!to dream up
+- (thông tục) tưởng tượng ra, bịa ra
+</t>
+  </si>
+  <si>
+    <t>youth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@youth /ju:θ/
+*  danh từ
+- tuổi trẻ, tuổi xuân, tuổi thanh niên, tuổi niên thiếu
+=the days of youth+ thời kỳ niên thiếu
+=from youth upwards+ từ lúc còn trẻ, từ nhỏ
+=the enthusiasm of youth+ nhiệt tình của tuổi trẻ
+- (nghĩa bóng) buổi ban đầu; thời non trẻ
+=the youth of civilization+ buổi ban đầu của nền văn minh
+=the youth of a nation+ thời kỳ non trẻ của một quốc gia
+- thanh niên; tầng lớp thanh niên, lứa tuổi thanh niên
+=a promising youth+ một thanh niên đầy hứa hẹn
+=a bevy of youths+ một đám thanh niên
+=the youth of one country+ lứa tuổi thanh niên của một nước
+=The Communist Youth League+ Đoàn thanh niên cộng sản
+=The Ho Chi Minh Labour Youth Union+ Đoàn thanh niên lao động Hồ Chí Minh
+</t>
   </si>
 </sst>
 </file>
@@ -449,7 +1037,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FA89061-8BF6-44C5-AC42-B85CC71C0DCE}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
@@ -478,6 +1066,388 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="331.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="345.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="216" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="331.2" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>